<commit_message>
understand how stage works
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>dafs</t>
   </si>
@@ -69,13 +69,22 @@
   </si>
   <si>
     <t>sadfsadf</t>
+  </si>
+  <si>
+    <t>dfsfad</t>
+  </si>
+  <si>
+    <t>dsfafsda</t>
+  </si>
+  <si>
+    <t>sdafsf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,13 +92,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,8 +138,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,18 +504,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="G16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -485,7 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E6:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>